<commit_message>
SK - Minimize and simplify the code structure
</commit_message>
<xml_diff>
--- a/Knockout Matrix Template_FILLED.xlsx
+++ b/Knockout Matrix Template_FILLED.xlsx
@@ -2051,7 +2051,7 @@
       </c>
       <c r="M30" s="28" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>YES, outstanding: 30667835.0, limit: 34070376.0</t>
         </is>
       </c>
       <c r="N30" s="5" t="n"/>
@@ -2085,7 +2085,11 @@
           <t>&gt; 2 times MIA2 for past 6 months and /or current 1 month &gt; 4 times MIA1</t>
         </is>
       </c>
-      <c r="M31" s="27" t="n"/>
+      <c r="M31" s="27" t="inlineStr">
+        <is>
+          <t>current 1 month MIA1: 7, MIA2: 0, MIA3: 0, MIA4+: 0 and /or past 6 months MIA1: 12, MIA2: 0, MIA3: 0, MIA4+: 0</t>
+        </is>
+      </c>
       <c r="N31" s="5" t="n"/>
       <c r="O31" s="27" t="n"/>
       <c r="P31" s="5" t="n"/>
@@ -2171,7 +2175,7 @@
       </c>
       <c r="M34" s="27" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>current 1 month MIA1: 0, MIA2: 0, MIA3: 0, MIA4+: 2 and /or past 6 months MIA1: 2, MIA2: 4, MIA3: 2, MIA4+: 4</t>
         </is>
       </c>
       <c r="N34" s="5" t="n"/>

</xml_diff>

<commit_message>
edit the keyword extractor
</commit_message>
<xml_diff>
--- a/Knockout Matrix Template_FILLED.xlsx
+++ b/Knockout Matrix Template_FILLED.xlsx
@@ -1298,7 +1298,7 @@
       </c>
       <c r="E6" s="7" t="inlineStr">
         <is>
-          <t>YOUR ISSUER SDN BHD</t>
+          <t>EVER FRESH CAMERON SDN. BHD.</t>
         </is>
       </c>
       <c r="F6" s="8" t="n"/>
@@ -1362,7 +1362,11 @@
           <t>Name</t>
         </is>
       </c>
-      <c r="M7" s="12" t="n"/>
+      <c r="M7" s="12" t="inlineStr">
+        <is>
+          <t>EVER FRESH CAMERON SDN. BHD.</t>
+        </is>
+      </c>
       <c r="N7" s="5" t="n"/>
       <c r="O7" s="13" t="n"/>
       <c r="P7" s="5" t="n"/>
@@ -1492,7 +1496,11 @@
           <t>No Score , E or worse</t>
         </is>
       </c>
-      <c r="M12" s="18" t="n"/>
+      <c r="M12" s="18" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
       <c r="N12" s="5" t="n"/>
       <c r="O12" s="18" t="n"/>
       <c r="P12" s="5" t="n"/>

</xml_diff>

<commit_message>
Sonnet CHanges to fill in the column
</commit_message>
<xml_diff>
--- a/Knockout Matrix Template_FILLED.xlsx
+++ b/Knockout Matrix Template_FILLED.xlsx
@@ -1368,9 +1368,27 @@
         </is>
       </c>
       <c r="N7" s="5" t="n"/>
-      <c r="O7" s="13" t="n"/>
+      <c r="O7" s="13" t="inlineStr">
+        <is>
+          <t>LAU HEE WOOI</t>
+        </is>
+      </c>
       <c r="P7" s="5" t="n"/>
-      <c r="Q7" s="13" t="n"/>
+      <c r="Q7" s="13" t="inlineStr">
+        <is>
+          <t>LAU HOOI MENG</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>LOH POEY CHUAN</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>LOH POEY CHUAN</t>
+        </is>
+      </c>
     </row>
     <row r="8" ht="17.1" customFormat="1" customHeight="1" s="2">
       <c r="D8" s="6" t="inlineStr">
@@ -1477,6 +1495,16 @@
           <t>644</t>
         </is>
       </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>575</t>
+        </is>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>575</t>
+        </is>
+      </c>
       <c r="V11" s="19" t="inlineStr">
         <is>
           <t>Issuer</t>
@@ -1514,9 +1542,27 @@
         </is>
       </c>
       <c r="N12" s="5" t="n"/>
-      <c r="O12" s="18" t="n"/>
+      <c r="O12" s="18" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
       <c r="P12" s="5" t="n"/>
-      <c r="Q12" s="18" t="n"/>
+      <c r="Q12" s="18" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
       <c r="V12" s="19" t="inlineStr">
         <is>
           <t>Director / Guarantor
@@ -1731,9 +1777,27 @@
         </is>
       </c>
       <c r="N18" s="5" t="n"/>
-      <c r="O18" s="18" t="n"/>
+      <c r="O18" s="18" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
       <c r="P18" s="5" t="n"/>
-      <c r="Q18" s="18" t="n"/>
+      <c r="Q18" s="18" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="19" ht="33.95" customFormat="1" customHeight="1" s="2">
       <c r="D19" s="129" t="inlineStr">
@@ -1759,9 +1823,27 @@
         </is>
       </c>
       <c r="N19" s="5" t="n"/>
-      <c r="O19" s="18" t="n"/>
+      <c r="O19" s="18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
       <c r="P19" s="5" t="n"/>
-      <c r="Q19" s="18" t="n"/>
+      <c r="Q19" s="18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="20" ht="17.1" customFormat="1" customHeight="1" s="2">
       <c r="D20" s="115" t="inlineStr">
@@ -1787,9 +1869,27 @@
         </is>
       </c>
       <c r="N20" s="5" t="n"/>
-      <c r="O20" s="18" t="n"/>
+      <c r="O20" s="18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
       <c r="P20" s="5" t="n"/>
-      <c r="Q20" s="18" t="n"/>
+      <c r="Q20" s="18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="21" ht="17.1" customFormat="1" customHeight="1" s="2">
       <c r="D21" s="115" t="inlineStr">
@@ -1815,9 +1915,27 @@
         </is>
       </c>
       <c r="N21" s="5" t="n"/>
-      <c r="O21" s="18" t="n"/>
+      <c r="O21" s="18" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
       <c r="P21" s="5" t="n"/>
-      <c r="Q21" s="18" t="n"/>
+      <c r="Q21" s="18" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U21" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="22" ht="17.1" customFormat="1" customHeight="1" s="2">
       <c r="D22" s="115" t="inlineStr">
@@ -1843,9 +1961,27 @@
         </is>
       </c>
       <c r="N22" s="5" t="n"/>
-      <c r="O22" s="18" t="n"/>
+      <c r="O22" s="18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
       <c r="P22" s="5" t="n"/>
-      <c r="Q22" s="18" t="n"/>
+      <c r="Q22" s="18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="23" ht="51" customFormat="1" customHeight="1" s="2">
       <c r="D23" s="115" t="inlineStr">
@@ -1867,13 +2003,31 @@
       </c>
       <c r="M23" s="27" t="inlineStr">
         <is>
-          <t>NoNoNo</t>
+          <t>Yes, Yes, No</t>
         </is>
       </c>
       <c r="N23" s="5" t="n"/>
-      <c r="O23" s="27" t="n"/>
+      <c r="O23" s="27" t="inlineStr">
+        <is>
+          <t>No, No, No</t>
+        </is>
+      </c>
       <c r="P23" s="5" t="n"/>
-      <c r="Q23" s="27" t="n"/>
+      <c r="Q23" s="27" t="inlineStr">
+        <is>
+          <t>No, No, No</t>
+        </is>
+      </c>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>No, No, No</t>
+        </is>
+      </c>
+      <c r="U23" t="inlineStr">
+        <is>
+          <t>No, No, No</t>
+        </is>
+      </c>
     </row>
     <row r="24" ht="17.1" customFormat="1" customHeight="1" s="2">
       <c r="D24" s="115" t="inlineStr">
@@ -1893,11 +2047,7 @@
           <t>&gt;1 &amp; outstanding &gt;RM10k</t>
         </is>
       </c>
-      <c r="M24" s="18" t="inlineStr">
-        <is>
-          <t>1127320.59</t>
-        </is>
-      </c>
+      <c r="M24" s="18" t="n"/>
       <c r="N24" s="5" t="n"/>
       <c r="O24" s="18" t="n"/>
       <c r="P24" s="5" t="n"/>
@@ -1927,9 +2077,27 @@
         </is>
       </c>
       <c r="N25" s="5" t="n"/>
-      <c r="O25" s="18" t="n"/>
+      <c r="O25" s="18" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
       <c r="P25" s="5" t="n"/>
-      <c r="Q25" s="18" t="n"/>
+      <c r="Q25" s="18" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="S25" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="U25" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
     </row>
     <row r="26" ht="20.1" customFormat="1" customHeight="1" s="2">
       <c r="D26" s="115" t="inlineStr">
@@ -1955,9 +2123,27 @@
         </is>
       </c>
       <c r="N26" s="5" t="n"/>
-      <c r="O26" s="18" t="n"/>
+      <c r="O26" s="18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
       <c r="P26" s="5" t="n"/>
-      <c r="Q26" s="18" t="n"/>
+      <c r="Q26" s="18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S26" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U26" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="27" ht="20.1" customFormat="1" customHeight="1" s="2">
       <c r="D27" s="115" t="inlineStr">
@@ -1983,9 +2169,27 @@
         </is>
       </c>
       <c r="N27" s="5" t="n"/>
-      <c r="O27" s="28" t="n"/>
+      <c r="O27" s="28" t="inlineStr">
+        <is>
+          <t>1349839</t>
+        </is>
+      </c>
       <c r="P27" s="5" t="n"/>
-      <c r="Q27" s="28" t="n"/>
+      <c r="Q27" s="28" t="inlineStr">
+        <is>
+          <t>1278562</t>
+        </is>
+      </c>
+      <c r="S27" t="inlineStr">
+        <is>
+          <t>17053</t>
+        </is>
+      </c>
+      <c r="U27" t="inlineStr">
+        <is>
+          <t>17053</t>
+        </is>
+      </c>
     </row>
     <row r="28" ht="20.1" customFormat="1" customHeight="1" s="2">
       <c r="D28" s="115" t="inlineStr">
@@ -2011,9 +2215,27 @@
         </is>
       </c>
       <c r="N28" s="5" t="n"/>
-      <c r="O28" s="28" t="n"/>
+      <c r="O28" s="28" t="inlineStr">
+        <is>
+          <t>1669243</t>
+        </is>
+      </c>
       <c r="P28" s="5" t="n"/>
-      <c r="Q28" s="28" t="n"/>
+      <c r="Q28" s="28" t="inlineStr">
+        <is>
+          <t>1707145</t>
+        </is>
+      </c>
+      <c r="S28" t="inlineStr">
+        <is>
+          <t>40000</t>
+        </is>
+      </c>
+      <c r="U28" t="inlineStr">
+        <is>
+          <t>40000</t>
+        </is>
+      </c>
     </row>
     <row r="29" ht="34.5" customFormat="1" customHeight="1" s="2">
       <c r="D29" s="115" t="inlineStr">
@@ -2041,13 +2263,23 @@
       <c r="N29" s="5" t="n"/>
       <c r="O29" s="24" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>No</t>
         </is>
       </c>
       <c r="P29" s="5" t="n"/>
       <c r="Q29" s="24" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S29" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="U29" t="inlineStr">
+        <is>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -2077,13 +2309,23 @@
       <c r="N30" s="5" t="n"/>
       <c r="O30" s="24" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>YES, outstanding: 30667835.0, limit: 34070376.0</t>
         </is>
       </c>
       <c r="P30" s="5" t="n"/>
       <c r="Q30" s="24" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>YES, outstanding: 30667835.0, limit: 34070376.0</t>
+        </is>
+      </c>
+      <c r="S30" t="inlineStr">
+        <is>
+          <t>YES, outstanding: 30667835.0, limit: 34070376.0</t>
+        </is>
+      </c>
+      <c r="U30" t="inlineStr">
+        <is>
+          <t>YES, outstanding: 30667835.0, limit: 34070376.0</t>
         </is>
       </c>
     </row>
@@ -2107,13 +2349,31 @@
       </c>
       <c r="M31" s="27" t="inlineStr">
         <is>
-          <t>current 1 month MIA1: 7, MIA2: 0, MIA3: 0, MIA4+: 0 and /or past 6 months MIA1: 12, MIA2: 0, MIA3: 0, MIA4+: 0</t>
+          <t>current 1 month MIA1: 34, MIA2: 0, MIA3: 1, MIA4+: 0 and /or past 6 months MIA1: 61, MIA2: 0, MIA3: 2, MIA4+: 0</t>
         </is>
       </c>
       <c r="N31" s="5" t="n"/>
-      <c r="O31" s="27" t="n"/>
+      <c r="O31" s="27" t="inlineStr">
+        <is>
+          <t>current 1 month MIA1: 34, MIA2: 0, MIA3: 1, MIA4+: 0 and /or past 6 months MIA1: 61, MIA2: 0, MIA3: 2, MIA4+: 0</t>
+        </is>
+      </c>
       <c r="P31" s="5" t="n"/>
-      <c r="Q31" s="27" t="n"/>
+      <c r="Q31" s="27" t="inlineStr">
+        <is>
+          <t>current 1 month MIA1: 34, MIA2: 0, MIA3: 1, MIA4+: 0 and /or past 6 months MIA1: 61, MIA2: 0, MIA3: 2, MIA4+: 0</t>
+        </is>
+      </c>
+      <c r="S31" t="inlineStr">
+        <is>
+          <t>current 1 month MIA1: 34, MIA2: 0, MIA3: 1, MIA4+: 0 and /or past 6 months MIA1: 61, MIA2: 0, MIA3: 2, MIA4+: 0</t>
+        </is>
+      </c>
+      <c r="U31" t="inlineStr">
+        <is>
+          <t>current 1 month MIA1: 34, MIA2: 0, MIA3: 1, MIA4+: 0 and /or past 6 months MIA1: 61, MIA2: 0, MIA3: 2, MIA4+: 0</t>
+        </is>
+      </c>
     </row>
     <row r="32" ht="20.1" customFormat="1" customHeight="1" s="2">
       <c r="D32" s="115" t="inlineStr">
@@ -2165,13 +2425,23 @@
       <c r="N33" s="5" t="n"/>
       <c r="O33" s="24" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="P33" s="5" t="n"/>
       <c r="Q33" s="24" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="S33" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="U33" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -2199,9 +2469,27 @@
         </is>
       </c>
       <c r="N34" s="5" t="n"/>
-      <c r="O34" s="27" t="n"/>
+      <c r="O34" s="27" t="inlineStr">
+        <is>
+          <t>current 1 month MIA1: 0, MIA2: 0, MIA3: 0, MIA4+: 2 and /or past 6 months MIA1: 2, MIA2: 4, MIA3: 2, MIA4+: 4</t>
+        </is>
+      </c>
       <c r="P34" s="5" t="n"/>
-      <c r="Q34" s="27" t="n"/>
+      <c r="Q34" s="27" t="inlineStr">
+        <is>
+          <t>current 1 month MIA1: 0, MIA2: 0, MIA3: 0, MIA4+: 2 and /or past 6 months MIA1: 2, MIA2: 4, MIA3: 2, MIA4+: 4</t>
+        </is>
+      </c>
+      <c r="S34" t="inlineStr">
+        <is>
+          <t>current 1 month MIA1: 0, MIA2: 0, MIA3: 0, MIA4+: 2 and /or past 6 months MIA1: 2, MIA2: 4, MIA3: 2, MIA4+: 4</t>
+        </is>
+      </c>
+      <c r="U34" t="inlineStr">
+        <is>
+          <t>current 1 month MIA1: 0, MIA2: 0, MIA3: 0, MIA4+: 2 and /or past 6 months MIA1: 2, MIA2: 4, MIA3: 2, MIA4+: 4</t>
+        </is>
+      </c>
     </row>
     <row r="35" ht="20.1" customFormat="1" customHeight="1" s="2">
       <c r="D35" s="115" t="inlineStr">
@@ -2227,9 +2515,27 @@
         </is>
       </c>
       <c r="N35" s="5" t="n"/>
-      <c r="O35" s="27" t="n"/>
+      <c r="O35" s="27" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
       <c r="P35" s="5" t="n"/>
-      <c r="Q35" s="27" t="n"/>
+      <c r="Q35" s="27" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="S35" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="U35" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
     </row>
     <row r="36" ht="33.95" customFormat="1" customHeight="1" s="2">
       <c r="D36" s="129" t="inlineStr">

</xml_diff>

<commit_message>
Sonnet insert the MIA into excel
</commit_message>
<xml_diff>
--- a/Knockout Matrix Template_FILLED.xlsx
+++ b/Knockout Matrix Template_FILLED.xlsx
@@ -2047,11 +2047,33 @@
           <t>&gt;1 &amp; outstanding &gt;RM10k</t>
         </is>
       </c>
-      <c r="M24" s="18" t="n"/>
+      <c r="M24" s="18" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
       <c r="N24" s="5" t="n"/>
-      <c r="O24" s="18" t="n"/>
+      <c r="O24" s="18" t="inlineStr">
+        <is>
+          <t>[214083.27, 141999.98]</t>
+        </is>
+      </c>
       <c r="P24" s="5" t="n"/>
-      <c r="Q24" s="18" t="n"/>
+      <c r="Q24" s="18" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="S24" t="inlineStr">
+        <is>
+          <t>[214083.27]</t>
+        </is>
+      </c>
+      <c r="U24" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
     </row>
     <row r="25" ht="17.1" customFormat="1" customHeight="1" s="2">
       <c r="D25" s="115" t="inlineStr">
@@ -2355,23 +2377,23 @@
       <c r="N31" s="5" t="n"/>
       <c r="O31" s="27" t="inlineStr">
         <is>
-          <t>current 1 month MIA1: 34, MIA2: 0, MIA3: 1, MIA4+: 0 and /or past 6 months MIA1: 61, MIA2: 0, MIA3: 2, MIA4+: 0</t>
+          <t>current 1 month MIA1: 4, MIA2: 0, MIA3: 0, MIA4+: 0 and /or past 6 months MIA1: 10, MIA2: 1, MIA3: 0, MIA4+: 0</t>
         </is>
       </c>
       <c r="P31" s="5" t="n"/>
       <c r="Q31" s="27" t="inlineStr">
         <is>
-          <t>current 1 month MIA1: 34, MIA2: 0, MIA3: 1, MIA4+: 0 and /or past 6 months MIA1: 61, MIA2: 0, MIA3: 2, MIA4+: 0</t>
+          <t>current 1 month MIA1: 1, MIA2: 0, MIA3: 0, MIA4+: 0 and /or past 6 months MIA1: 8, MIA2: 0, MIA3: 0, MIA4+: 0</t>
         </is>
       </c>
       <c r="S31" t="inlineStr">
         <is>
-          <t>current 1 month MIA1: 34, MIA2: 0, MIA3: 1, MIA4+: 0 and /or past 6 months MIA1: 61, MIA2: 0, MIA3: 2, MIA4+: 0</t>
+          <t>current 1 month MIA1: 0, MIA2: 0, MIA3: 0, MIA4+: 0 and /or past 6 months MIA1: 0, MIA2: 0, MIA3: 0, MIA4+: 0</t>
         </is>
       </c>
       <c r="U31" t="inlineStr">
         <is>
-          <t>current 1 month MIA1: 34, MIA2: 0, MIA3: 1, MIA4+: 0 and /or past 6 months MIA1: 61, MIA2: 0, MIA3: 2, MIA4+: 0</t>
+          <t>current 1 month MIA1: 0, MIA2: 0, MIA3: 0, MIA4+: 0 and /or past 6 months MIA1: 0, MIA2: 0, MIA3: 0, MIA4+: 0</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Kian Hou requested changes
</commit_message>
<xml_diff>
--- a/Knockout Matrix Template_FILLED.xlsx
+++ b/Knockout Matrix Template_FILLED.xlsx
@@ -1298,7 +1298,7 @@
       </c>
       <c r="E6" s="7" t="inlineStr">
         <is>
-          <t>ZATIKIMIA SDN. BHD.</t>
+          <t>EVER FRESH CAMERON SDN. BHD.</t>
         </is>
       </c>
       <c r="F6" s="8" t="n"/>
@@ -1353,7 +1353,7 @@
       </c>
       <c r="J7" s="7" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-10-28</t>
         </is>
       </c>
       <c r="K7" s="8" t="n"/>
@@ -1364,15 +1364,11 @@
       </c>
       <c r="M7" s="12" t="inlineStr">
         <is>
-          <t>ZATIKIMIA SDN. BHD.</t>
+          <t>EVER FRESH CAMERON SDN. BHD.</t>
         </is>
       </c>
       <c r="N7" s="5" t="n"/>
-      <c r="O7" s="13" t="inlineStr">
-        <is>
-          <t>NORHAYATI BINTI HASHIM</t>
-        </is>
-      </c>
+      <c r="O7" s="13" t="n"/>
       <c r="P7" s="5" t="n"/>
       <c r="Q7" s="13" t="n"/>
     </row>
@@ -1462,17 +1458,31 @@
       <c r="L11" s="17" t="n"/>
       <c r="M11" s="18" t="inlineStr">
         <is>
-          <t>462</t>
+          <t>300</t>
         </is>
       </c>
       <c r="N11" s="5" t="n"/>
       <c r="O11" s="18" t="inlineStr">
         <is>
-          <t>582</t>
+          <t>543</t>
         </is>
       </c>
       <c r="P11" s="5" t="n"/>
-      <c r="Q11" s="18" t="n"/>
+      <c r="Q11" s="18" t="inlineStr">
+        <is>
+          <t>644</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>575</t>
+        </is>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>575</t>
+        </is>
+      </c>
       <c r="V11" s="19" t="inlineStr">
         <is>
           <t>Issuer</t>
@@ -1506,7 +1516,7 @@
       </c>
       <c r="M12" s="18" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>F</t>
         </is>
       </c>
       <c r="N12" s="5" t="n"/>
@@ -1516,7 +1526,21 @@
         </is>
       </c>
       <c r="P12" s="5" t="n"/>
-      <c r="Q12" s="18" t="n"/>
+      <c r="Q12" s="18" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
       <c r="V12" s="19" t="inlineStr">
         <is>
           <t>Director / Guarantor
@@ -1548,7 +1572,7 @@
       </c>
       <c r="M13" s="23" t="inlineStr">
         <is>
-          <t>2000</t>
+          <t>2013</t>
         </is>
       </c>
       <c r="N13" s="5" t="n"/>
@@ -1733,11 +1757,25 @@
       <c r="N18" s="5" t="n"/>
       <c r="O18" s="18" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3</t>
         </is>
       </c>
       <c r="P18" s="5" t="n"/>
-      <c r="Q18" s="18" t="n"/>
+      <c r="Q18" s="18" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="19" ht="33.95" customFormat="1" customHeight="1" s="2">
       <c r="D19" s="129" t="inlineStr">
@@ -1769,7 +1807,21 @@
         </is>
       </c>
       <c r="P19" s="5" t="n"/>
-      <c r="Q19" s="18" t="n"/>
+      <c r="Q19" s="18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="20" ht="17.1" customFormat="1" customHeight="1" s="2">
       <c r="D20" s="115" t="inlineStr">
@@ -1801,7 +1853,21 @@
         </is>
       </c>
       <c r="P20" s="5" t="n"/>
-      <c r="Q20" s="18" t="n"/>
+      <c r="Q20" s="18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="21" ht="17.1" customFormat="1" customHeight="1" s="2">
       <c r="D21" s="115" t="inlineStr">
@@ -1823,17 +1889,31 @@
       </c>
       <c r="M21" s="18" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>35</t>
         </is>
       </c>
       <c r="N21" s="5" t="n"/>
       <c r="O21" s="18" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>11</t>
         </is>
       </c>
       <c r="P21" s="5" t="n"/>
-      <c r="Q21" s="18" t="n"/>
+      <c r="Q21" s="18" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U21" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="22" ht="17.1" customFormat="1" customHeight="1" s="2">
       <c r="D22" s="115" t="inlineStr">
@@ -1855,17 +1935,31 @@
       </c>
       <c r="M22" s="18" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
       <c r="N22" s="5" t="n"/>
       <c r="O22" s="18" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="P22" s="5" t="n"/>
-      <c r="Q22" s="18" t="n"/>
+      <c r="Q22" s="18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="23" ht="51" customFormat="1" customHeight="1" s="2">
       <c r="D23" s="115" t="inlineStr">
@@ -1887,17 +1981,31 @@
       </c>
       <c r="M23" s="27" t="inlineStr">
         <is>
-          <t>No, Yes, Yes</t>
+          <t>Yes, Yes, No</t>
         </is>
       </c>
       <c r="N23" s="5" t="n"/>
       <c r="O23" s="27" t="inlineStr">
         <is>
-          <t>No, No, Yes</t>
+          <t>No, No, No</t>
         </is>
       </c>
       <c r="P23" s="5" t="n"/>
-      <c r="Q23" s="27" t="n"/>
+      <c r="Q23" s="27" t="inlineStr">
+        <is>
+          <t>No, No, No</t>
+        </is>
+      </c>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>No, No, No</t>
+        </is>
+      </c>
+      <c r="U23" t="inlineStr">
+        <is>
+          <t>No, No, No</t>
+        </is>
+      </c>
     </row>
     <row r="24" ht="17.1" customFormat="1" customHeight="1" s="2">
       <c r="D24" s="115" t="inlineStr">
@@ -1917,11 +2025,33 @@
           <t>&gt;1 &amp; outstanding &gt;RM10k</t>
         </is>
       </c>
-      <c r="M24" s="18" t="n"/>
+      <c r="M24" s="18" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
       <c r="N24" s="5" t="n"/>
-      <c r="O24" s="18" t="n"/>
+      <c r="O24" s="18" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
       <c r="P24" s="5" t="n"/>
-      <c r="Q24" s="18" t="n"/>
+      <c r="Q24" s="18" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="S24" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="U24" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
     </row>
     <row r="25" ht="17.1" customFormat="1" customHeight="1" s="2">
       <c r="D25" s="115" t="inlineStr">
@@ -1949,11 +2079,25 @@
       <c r="N25" s="5" t="n"/>
       <c r="O25" s="18" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
       <c r="P25" s="5" t="n"/>
-      <c r="Q25" s="18" t="n"/>
+      <c r="Q25" s="18" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="S25" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="U25" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
     </row>
     <row r="26" ht="20.1" customFormat="1" customHeight="1" s="2">
       <c r="D26" s="115" t="inlineStr">
@@ -1985,7 +2129,21 @@
         </is>
       </c>
       <c r="P26" s="5" t="n"/>
-      <c r="Q26" s="18" t="n"/>
+      <c r="Q26" s="18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S26" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U26" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="27" ht="20.1" customFormat="1" customHeight="1" s="2">
       <c r="D27" s="115" t="inlineStr">
@@ -2007,17 +2165,31 @@
       </c>
       <c r="M27" s="28" t="inlineStr">
         <is>
-          <t>787576</t>
+          <t>30667835</t>
         </is>
       </c>
       <c r="N27" s="5" t="n"/>
       <c r="O27" s="28" t="inlineStr">
         <is>
-          <t>525623</t>
+          <t>1349839</t>
         </is>
       </c>
       <c r="P27" s="5" t="n"/>
-      <c r="Q27" s="28" t="n"/>
+      <c r="Q27" s="28" t="inlineStr">
+        <is>
+          <t>1278562</t>
+        </is>
+      </c>
+      <c r="S27" t="inlineStr">
+        <is>
+          <t>17053</t>
+        </is>
+      </c>
+      <c r="U27" t="inlineStr">
+        <is>
+          <t>17053</t>
+        </is>
+      </c>
     </row>
     <row r="28" ht="20.1" customFormat="1" customHeight="1" s="2">
       <c r="D28" s="115" t="inlineStr">
@@ -2039,17 +2211,31 @@
       </c>
       <c r="M28" s="28" t="inlineStr">
         <is>
-          <t>990000</t>
+          <t>34070376</t>
         </is>
       </c>
       <c r="N28" s="5" t="n"/>
       <c r="O28" s="28" t="inlineStr">
         <is>
-          <t>780000</t>
+          <t>1669243</t>
         </is>
       </c>
       <c r="P28" s="5" t="n"/>
-      <c r="Q28" s="28" t="n"/>
+      <c r="Q28" s="28" t="inlineStr">
+        <is>
+          <t>1707145</t>
+        </is>
+      </c>
+      <c r="S28" t="inlineStr">
+        <is>
+          <t>40000</t>
+        </is>
+      </c>
+      <c r="U28" t="inlineStr">
+        <is>
+          <t>40000</t>
+        </is>
+      </c>
     </row>
     <row r="29" ht="34.5" customFormat="1" customHeight="1" s="2">
       <c r="D29" s="115" t="inlineStr">
@@ -2083,7 +2269,17 @@
       <c r="P29" s="5" t="n"/>
       <c r="Q29" s="24" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S29" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="U29" t="inlineStr">
+        <is>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -2107,19 +2303,29 @@
       </c>
       <c r="M30" s="28" t="inlineStr">
         <is>
-          <t>YES, outstanding: 787576.0, limit: 990000.0</t>
+          <t>YES, outstanding: 30667835.0, limit: 34070376.0</t>
         </is>
       </c>
       <c r="N30" s="5" t="n"/>
       <c r="O30" s="24" t="inlineStr">
         <is>
-          <t>YES, outstanding: 787576.0, limit: 990000.0</t>
+          <t>YES, outstanding: 30667835.0, limit: 34070376.0</t>
         </is>
       </c>
       <c r="P30" s="5" t="n"/>
       <c r="Q30" s="24" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>YES, outstanding: 30667835.0, limit: 34070376.0</t>
+        </is>
+      </c>
+      <c r="S30" t="inlineStr">
+        <is>
+          <t>YES, outstanding: 30667835.0, limit: 34070376.0</t>
+        </is>
+      </c>
+      <c r="U30" t="inlineStr">
+        <is>
+          <t>YES, outstanding: 30667835.0, limit: 34070376.0</t>
         </is>
       </c>
     </row>
@@ -2143,17 +2349,31 @@
       </c>
       <c r="M31" s="27" t="inlineStr">
         <is>
-          <t>current 1 month MIA1: 0, MIA2: 0, MIA3: 0, MIA4+: 0 and /or past 6 months MIA1: 3, MIA2: 3, MIA3: 0, MIA4+: 0</t>
+          <t>current 1 month MIA1: 34, MIA2: 0, MIA3: 1, MIA4+: 0 and /or past 6 months MIA1: 61, MIA2: 0, MIA3: 2, MIA4+: 0</t>
         </is>
       </c>
       <c r="N31" s="5" t="n"/>
       <c r="O31" s="27" t="inlineStr">
         <is>
-          <t>current 1 month MIA1: 0, MIA2: 0, MIA3: 0, MIA4+: 0 and /or past 6 months MIA1: 12, MIA2: 13, MIA3: 0, MIA4+: 0</t>
+          <t>current 1 month MIA1: 4, MIA2: 0, MIA3: 0, MIA4+: 0 and /or past 6 months MIA1: 10, MIA2: 1, MIA3: 0, MIA4+: 0</t>
         </is>
       </c>
       <c r="P31" s="5" t="n"/>
-      <c r="Q31" s="27" t="n"/>
+      <c r="Q31" s="27" t="inlineStr">
+        <is>
+          <t>current 1 month MIA1: 1, MIA2: 0, MIA3: 0, MIA4+: 0 and /or past 6 months MIA1: 8, MIA2: 0, MIA3: 0, MIA4+: 0</t>
+        </is>
+      </c>
+      <c r="S31" t="inlineStr">
+        <is>
+          <t>current 1 month MIA1: 0, MIA2: 0, MIA3: 0, MIA4+: 0 and /or past 6 months MIA1: 0, MIA2: 0, MIA3: 0, MIA4+: 0</t>
+        </is>
+      </c>
+      <c r="U31" t="inlineStr">
+        <is>
+          <t>current 1 month MIA1: 0, MIA2: 0, MIA3: 0, MIA4+: 0 and /or past 6 months MIA1: 0, MIA2: 0, MIA3: 0, MIA4+: 0</t>
+        </is>
+      </c>
     </row>
     <row r="32" ht="20.1" customFormat="1" customHeight="1" s="2">
       <c r="D32" s="115" t="inlineStr">
@@ -2211,7 +2431,17 @@
       <c r="P33" s="5" t="n"/>
       <c r="Q33" s="24" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="S33" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="U33" t="inlineStr">
+        <is>
+          <t>NO</t>
         </is>
       </c>
     </row>
@@ -2235,17 +2465,31 @@
       </c>
       <c r="M34" s="27" t="inlineStr">
         <is>
-          <t>current 1 month MIA1: 0, MIA2: 0, MIA3: 0, MIA4+: 0 and /or past 6 months MIA1: 0, MIA2: 0, MIA3: 0, MIA4+: 0</t>
+          <t>current 1 month MIA1: 0, MIA2: 0, MIA3: 0, MIA4+: 2 and /or past 6 months MIA1: 2, MIA2: 4, MIA3: 2, MIA4+: 4</t>
         </is>
       </c>
       <c r="N34" s="5" t="n"/>
       <c r="O34" s="27" t="inlineStr">
         <is>
-          <t>current 1 month MIA1: 0, MIA2: 0, MIA3: 0, MIA4+: 0 and /or past 6 months MIA1: 0, MIA2: 0, MIA3: 0, MIA4+: 0</t>
+          <t>current 1 month MIA1: 0, MIA2: 0, MIA3: 0, MIA4+: 2 and /or past 6 months MIA1: 2, MIA2: 4, MIA3: 2, MIA4+: 4</t>
         </is>
       </c>
       <c r="P34" s="5" t="n"/>
-      <c r="Q34" s="27" t="n"/>
+      <c r="Q34" s="27" t="inlineStr">
+        <is>
+          <t>current 1 month MIA1: 0, MIA2: 0, MIA3: 0, MIA4+: 2 and /or past 6 months MIA1: 2, MIA2: 4, MIA3: 2, MIA4+: 4</t>
+        </is>
+      </c>
+      <c r="S34" t="inlineStr">
+        <is>
+          <t>current 1 month MIA1: 0, MIA2: 0, MIA3: 0, MIA4+: 2 and /or past 6 months MIA1: 2, MIA2: 4, MIA3: 2, MIA4+: 4</t>
+        </is>
+      </c>
+      <c r="U34" t="inlineStr">
+        <is>
+          <t>current 1 month MIA1: 0, MIA2: 0, MIA3: 0, MIA4+: 2 and /or past 6 months MIA1: 2, MIA2: 4, MIA3: 2, MIA4+: 4</t>
+        </is>
+      </c>
     </row>
     <row r="35" ht="20.1" customFormat="1" customHeight="1" s="2">
       <c r="D35" s="115" t="inlineStr">
@@ -2267,17 +2511,31 @@
       </c>
       <c r="M35" s="18" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>LOD</t>
         </is>
       </c>
       <c r="N35" s="5" t="n"/>
       <c r="O35" s="27" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>LOD</t>
         </is>
       </c>
       <c r="P35" s="5" t="n"/>
-      <c r="Q35" s="27" t="n"/>
+      <c r="Q35" s="27" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="S35" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
+      <c r="U35" t="inlineStr">
+        <is>
+          <t>LOD</t>
+        </is>
+      </c>
     </row>
     <row r="36" ht="33.95" customFormat="1" customHeight="1" s="2">
       <c r="D36" s="129" t="inlineStr">

</xml_diff>

<commit_message>
Kian Hou - Fixed the MIA 4
</commit_message>
<xml_diff>
--- a/Knockout Matrix Template_FILLED.xlsx
+++ b/Knockout Matrix Template_FILLED.xlsx
@@ -1298,7 +1298,7 @@
       </c>
       <c r="E6" s="7" t="inlineStr">
         <is>
-          <t>EVER FRESH CAMERON SDN. BHD.</t>
+          <t>GREATOCEAN AUTOMOBILE SUPPLY SDN. BHD.</t>
         </is>
       </c>
       <c r="F6" s="8" t="n"/>
@@ -1353,7 +1353,7 @@
       </c>
       <c r="J7" s="7" t="inlineStr">
         <is>
-          <t>2025-10-28</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="K7" s="8" t="n"/>
@@ -1364,7 +1364,7 @@
       </c>
       <c r="M7" s="12" t="inlineStr">
         <is>
-          <t>EVER FRESH CAMERON SDN. BHD.</t>
+          <t>GREATOCEAN AUTOMOBILE SUPPLY SDN. BHD.</t>
         </is>
       </c>
       <c r="N7" s="5" t="n"/>
@@ -1458,29 +1458,19 @@
       <c r="L11" s="17" t="n"/>
       <c r="M11" s="18" t="inlineStr">
         <is>
-          <t>300</t>
+          <t>678</t>
         </is>
       </c>
       <c r="N11" s="5" t="n"/>
       <c r="O11" s="18" t="inlineStr">
         <is>
-          <t>543</t>
+          <t>311</t>
         </is>
       </c>
       <c r="P11" s="5" t="n"/>
       <c r="Q11" s="18" t="inlineStr">
         <is>
-          <t>644</t>
-        </is>
-      </c>
-      <c r="S11" t="inlineStr">
-        <is>
-          <t>575</t>
-        </is>
-      </c>
-      <c r="U11" t="inlineStr">
-        <is>
-          <t>575</t>
+          <t>533</t>
         </is>
       </c>
       <c r="V11" s="19" t="inlineStr">
@@ -1516,29 +1506,19 @@
       </c>
       <c r="M12" s="18" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>B</t>
         </is>
       </c>
       <c r="N12" s="5" t="n"/>
       <c r="O12" s="18" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>F</t>
         </is>
       </c>
       <c r="P12" s="5" t="n"/>
       <c r="Q12" s="18" t="inlineStr">
         <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="S12" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="U12" t="inlineStr">
-        <is>
-          <t>C</t>
+          <t>D</t>
         </is>
       </c>
       <c r="V12" s="19" t="inlineStr">
@@ -1572,7 +1552,7 @@
       </c>
       <c r="M13" s="23" t="inlineStr">
         <is>
-          <t>2013</t>
+          <t>2011</t>
         </is>
       </c>
       <c r="N13" s="5" t="n"/>
@@ -1751,29 +1731,19 @@
       </c>
       <c r="M18" s="18" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="N18" s="5" t="n"/>
       <c r="O18" s="18" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0</t>
         </is>
       </c>
       <c r="P18" s="5" t="n"/>
       <c r="Q18" s="18" t="inlineStr">
         <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="S18" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="U18" t="inlineStr">
-        <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -1812,16 +1782,6 @@
           <t>0</t>
         </is>
       </c>
-      <c r="S19" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="U19" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
     </row>
     <row r="20" ht="17.1" customFormat="1" customHeight="1" s="2">
       <c r="D20" s="115" t="inlineStr">
@@ -1858,16 +1818,6 @@
           <t>0</t>
         </is>
       </c>
-      <c r="S20" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="U20" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
     </row>
     <row r="21" ht="17.1" customFormat="1" customHeight="1" s="2">
       <c r="D21" s="115" t="inlineStr">
@@ -1889,29 +1839,19 @@
       </c>
       <c r="M21" s="18" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>16</t>
         </is>
       </c>
       <c r="N21" s="5" t="n"/>
       <c r="O21" s="18" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>10</t>
         </is>
       </c>
       <c r="P21" s="5" t="n"/>
       <c r="Q21" s="18" t="inlineStr">
         <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="S21" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="U21" t="inlineStr">
-        <is>
-          <t>1</t>
+          <t>9</t>
         </is>
       </c>
     </row>
@@ -1935,7 +1875,7 @@
       </c>
       <c r="M22" s="18" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="N22" s="5" t="n"/>
@@ -1946,16 +1886,6 @@
       </c>
       <c r="P22" s="5" t="n"/>
       <c r="Q22" s="18" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="S22" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="U22" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1981,7 +1911,7 @@
       </c>
       <c r="M23" s="27" t="inlineStr">
         <is>
-          <t>Yes, Yes, No</t>
+          <t>No, No, No</t>
         </is>
       </c>
       <c r="N23" s="5" t="n"/>
@@ -1992,16 +1922,6 @@
       </c>
       <c r="P23" s="5" t="n"/>
       <c r="Q23" s="27" t="inlineStr">
-        <is>
-          <t>No, No, No</t>
-        </is>
-      </c>
-      <c r="S23" t="inlineStr">
-        <is>
-          <t>No, No, No</t>
-        </is>
-      </c>
-      <c r="U23" t="inlineStr">
         <is>
           <t>No, No, No</t>
         </is>
@@ -2025,33 +1945,11 @@
           <t>&gt;1 &amp; outstanding &gt;RM10k</t>
         </is>
       </c>
-      <c r="M24" s="18" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
+      <c r="M24" s="18" t="n"/>
       <c r="N24" s="5" t="n"/>
-      <c r="O24" s="18" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
+      <c r="O24" s="18" t="n"/>
       <c r="P24" s="5" t="n"/>
-      <c r="Q24" s="18" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="S24" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="U24" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
+      <c r="Q24" s="18" t="n"/>
     </row>
     <row r="25" ht="17.1" customFormat="1" customHeight="1" s="2">
       <c r="D25" s="115" t="inlineStr">
@@ -2073,27 +1971,17 @@
       </c>
       <c r="M25" s="18" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>4</t>
         </is>
       </c>
       <c r="N25" s="5" t="n"/>
       <c r="O25" s="18" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="P25" s="5" t="n"/>
       <c r="Q25" s="18" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="S25" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="U25" t="inlineStr">
         <is>
           <t>2</t>
         </is>
@@ -2134,16 +2022,6 @@
           <t>0</t>
         </is>
       </c>
-      <c r="S26" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="U26" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
     </row>
     <row r="27" ht="20.1" customFormat="1" customHeight="1" s="2">
       <c r="D27" s="115" t="inlineStr">
@@ -2165,29 +2043,19 @@
       </c>
       <c r="M27" s="28" t="inlineStr">
         <is>
-          <t>30667835</t>
+          <t>15436493</t>
         </is>
       </c>
       <c r="N27" s="5" t="n"/>
       <c r="O27" s="28" t="inlineStr">
         <is>
-          <t>1349839</t>
+          <t>1753657</t>
         </is>
       </c>
       <c r="P27" s="5" t="n"/>
       <c r="Q27" s="28" t="inlineStr">
         <is>
-          <t>1278562</t>
-        </is>
-      </c>
-      <c r="S27" t="inlineStr">
-        <is>
-          <t>17053</t>
-        </is>
-      </c>
-      <c r="U27" t="inlineStr">
-        <is>
-          <t>17053</t>
+          <t>1723015</t>
         </is>
       </c>
     </row>
@@ -2211,29 +2079,19 @@
       </c>
       <c r="M28" s="28" t="inlineStr">
         <is>
-          <t>34070376</t>
+          <t>16364987</t>
         </is>
       </c>
       <c r="N28" s="5" t="n"/>
       <c r="O28" s="28" t="inlineStr">
         <is>
-          <t>1669243</t>
+          <t>2146309</t>
         </is>
       </c>
       <c r="P28" s="5" t="n"/>
       <c r="Q28" s="28" t="inlineStr">
         <is>
-          <t>1707145</t>
-        </is>
-      </c>
-      <c r="S28" t="inlineStr">
-        <is>
-          <t>40000</t>
-        </is>
-      </c>
-      <c r="U28" t="inlineStr">
-        <is>
-          <t>40000</t>
+          <t>2094126</t>
         </is>
       </c>
     </row>
@@ -2272,16 +2130,6 @@
           <t>No</t>
         </is>
       </c>
-      <c r="S29" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="U29" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
     </row>
     <row r="30" ht="42" customFormat="1" customHeight="1" s="2">
       <c r="D30" s="115" t="inlineStr">
@@ -2303,29 +2151,19 @@
       </c>
       <c r="M30" s="28" t="inlineStr">
         <is>
-          <t>YES, outstanding: 30667835.0, limit: 34070376.0</t>
+          <t>YES, outstanding: 15520690.0, limit: 17714987.0</t>
         </is>
       </c>
       <c r="N30" s="5" t="n"/>
       <c r="O30" s="24" t="inlineStr">
         <is>
-          <t>YES, outstanding: 30667835.0, limit: 34070376.0</t>
+          <t>YES, outstanding: 15520690.0, limit: 17714987.0</t>
         </is>
       </c>
       <c r="P30" s="5" t="n"/>
       <c r="Q30" s="24" t="inlineStr">
         <is>
-          <t>YES, outstanding: 30667835.0, limit: 34070376.0</t>
-        </is>
-      </c>
-      <c r="S30" t="inlineStr">
-        <is>
-          <t>YES, outstanding: 30667835.0, limit: 34070376.0</t>
-        </is>
-      </c>
-      <c r="U30" t="inlineStr">
-        <is>
-          <t>YES, outstanding: 30667835.0, limit: 34070376.0</t>
+          <t>YES, outstanding: 15520690.0, limit: 17714987.0</t>
         </is>
       </c>
     </row>
@@ -2349,29 +2187,19 @@
       </c>
       <c r="M31" s="27" t="inlineStr">
         <is>
-          <t>current 1 month MIA1: 34, MIA2: 0, MIA3: 1, MIA4+: 0 and /or past 6 months MIA1: 61, MIA2: 0, MIA3: 2, MIA4+: 0</t>
+          <t>current 1 month MIA1: 1, MIA2: 0, MIA3: 0, MIA4+: 0 and /or past 6 months MIA1: 1, MIA2: 0, MIA3: 0, MIA4+: 0</t>
         </is>
       </c>
       <c r="N31" s="5" t="n"/>
       <c r="O31" s="27" t="inlineStr">
         <is>
-          <t>current 1 month MIA1: 4, MIA2: 0, MIA3: 0, MIA4+: 0 and /or past 6 months MIA1: 10, MIA2: 1, MIA3: 0, MIA4+: 0</t>
+          <t>current 1 month MIA1: 0, MIA2: 0, MIA3: 0, MIA4+: 1 and /or past 6 months MIA1: 1, MIA2: 1, MIA3: 1, MIA4+: 2</t>
         </is>
       </c>
       <c r="P31" s="5" t="n"/>
       <c r="Q31" s="27" t="inlineStr">
         <is>
-          <t>current 1 month MIA1: 1, MIA2: 0, MIA3: 0, MIA4+: 0 and /or past 6 months MIA1: 8, MIA2: 0, MIA3: 0, MIA4+: 0</t>
-        </is>
-      </c>
-      <c r="S31" t="inlineStr">
-        <is>
-          <t>current 1 month MIA1: 0, MIA2: 0, MIA3: 0, MIA4+: 0 and /or past 6 months MIA1: 0, MIA2: 0, MIA3: 0, MIA4+: 0</t>
-        </is>
-      </c>
-      <c r="U31" t="inlineStr">
-        <is>
-          <t>current 1 month MIA1: 0, MIA2: 0, MIA3: 0, MIA4+: 0 and /or past 6 months MIA1: 0, MIA2: 0, MIA3: 0, MIA4+: 0</t>
+          <t>current 1 month MIA1: 0, MIA2: 1, MIA3: 0, MIA4+: 0 and /or past 6 months MIA1: 6, MIA2: 3, MIA3: 1, MIA4+: 0</t>
         </is>
       </c>
     </row>
@@ -2434,16 +2262,6 @@
           <t>NO</t>
         </is>
       </c>
-      <c r="S33" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="U33" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
     </row>
     <row r="34" ht="58.5" customFormat="1" customHeight="1" s="2">
       <c r="D34" s="115" t="inlineStr">
@@ -2465,29 +2283,19 @@
       </c>
       <c r="M34" s="27" t="inlineStr">
         <is>
-          <t>current 1 month MIA1: 0, MIA2: 0, MIA3: 0, MIA4+: 2 and /or past 6 months MIA1: 2, MIA2: 4, MIA3: 2, MIA4+: 4</t>
+          <t>current 1 month MIA1: 0, MIA2: 0, MIA3: 0, MIA4+: 0 and /or past 6 months MIA1: 0, MIA2: 0, MIA3: 0, MIA4+: 0</t>
         </is>
       </c>
       <c r="N34" s="5" t="n"/>
       <c r="O34" s="27" t="inlineStr">
         <is>
-          <t>current 1 month MIA1: 0, MIA2: 0, MIA3: 0, MIA4+: 2 and /or past 6 months MIA1: 2, MIA2: 4, MIA3: 2, MIA4+: 4</t>
+          <t>current 1 month MIA1: 0, MIA2: 0, MIA3: 0, MIA4+: 0 and /or past 6 months MIA1: 0, MIA2: 0, MIA3: 0, MIA4+: 0</t>
         </is>
       </c>
       <c r="P34" s="5" t="n"/>
       <c r="Q34" s="27" t="inlineStr">
         <is>
-          <t>current 1 month MIA1: 0, MIA2: 0, MIA3: 0, MIA4+: 2 and /or past 6 months MIA1: 2, MIA2: 4, MIA3: 2, MIA4+: 4</t>
-        </is>
-      </c>
-      <c r="S34" t="inlineStr">
-        <is>
-          <t>current 1 month MIA1: 0, MIA2: 0, MIA3: 0, MIA4+: 2 and /or past 6 months MIA1: 2, MIA2: 4, MIA3: 2, MIA4+: 4</t>
-        </is>
-      </c>
-      <c r="U34" t="inlineStr">
-        <is>
-          <t>current 1 month MIA1: 0, MIA2: 0, MIA3: 0, MIA4+: 2 and /or past 6 months MIA1: 2, MIA2: 4, MIA3: 2, MIA4+: 4</t>
+          <t>current 1 month MIA1: 0, MIA2: 0, MIA3: 0, MIA4+: 0 and /or past 6 months MIA1: 0, MIA2: 0, MIA3: 0, MIA4+: 0</t>
         </is>
       </c>
     </row>
@@ -2511,29 +2319,19 @@
       </c>
       <c r="M35" s="18" t="inlineStr">
         <is>
-          <t>LOD</t>
+          <t>WITHDRAWN</t>
         </is>
       </c>
       <c r="N35" s="5" t="n"/>
       <c r="O35" s="27" t="inlineStr">
         <is>
-          <t>LOD</t>
+          <t>WITHDRAWN</t>
         </is>
       </c>
       <c r="P35" s="5" t="n"/>
       <c r="Q35" s="27" t="inlineStr">
         <is>
-          <t>LOD</t>
-        </is>
-      </c>
-      <c r="S35" t="inlineStr">
-        <is>
-          <t>LOD</t>
-        </is>
-      </c>
-      <c r="U35" t="inlineStr">
-        <is>
-          <t>LOD</t>
+          <t>WITHDRAWN</t>
         </is>
       </c>
     </row>

</xml_diff>